<commit_message>
Data preparation (excel files), implementation of the history management to map each procedures numbers to the last reviewed date, preparation of the unit tests
</commit_message>
<xml_diff>
--- a/data/Liste sujets discussions mensuelles.xlsx
+++ b/data/Liste sujets discussions mensuelles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bayergroup-my.sharepoint.com/personal/axel_cano_bayer_com/Documents/desktop/Axel/HSE/Discussions mensuelles de sécurité et vérification priodique/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bayergroup-my.sharepoint.com/personal/axel_cano_bayer_com/Documents/desktop/Axel/Code/Projets/byr_HSE_subjects/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{3CE83B51-2702-4B65-8362-F85B593A72EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE0A6C68-576A-44F6-BF35-DE9694A4C908}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{3CE83B51-2702-4B65-8362-F85B593A72EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59C65915-80C2-4CF2-86AD-FD7F838915BD}"/>
   <bookViews>
-    <workbookView xWindow="564" yWindow="1740" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="133">
   <si>
     <t>Procedure</t>
   </si>
@@ -430,9 +430,6 @@
     <t xml:space="preserve">Précurseurs de drogues </t>
   </si>
   <si>
-    <t xml:space="preserve">PROC16 </t>
-  </si>
-  <si>
     <t>Consignes de travail et de sécurité en laboratoire de synthèse</t>
   </si>
   <si>
@@ -509,6 +506,9 @@
   </si>
   <si>
     <t>Nouvelle procédure electrochimie</t>
+  </si>
+  <si>
+    <t>youtube</t>
   </si>
 </sst>
 </file>
@@ -955,19 +955,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.59765625" customWidth="1"/>
-    <col min="2" max="2" width="104.5" customWidth="1"/>
-    <col min="3" max="3" width="12.3984375" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.125" customWidth="1"/>
+    <col min="2" max="2" width="77" customWidth="1"/>
+    <col min="3" max="3" width="12.375" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -981,7 +981,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -995,7 +995,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>42826</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>42917</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>42979</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>43009</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>43070</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>43160</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>43191</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>43221</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>43252</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>43282</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>43405</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>43435</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>43497</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>43556</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>43647</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>43709</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>43739</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>82</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>43770</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>43831</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>43891</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>64</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>43952</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>43983</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>84</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>44105</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>51</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>44136</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>86</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>67</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>44197</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>68</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>70</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>44256</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>73</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>44287</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>75</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>44317</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>76</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>44348</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>44378</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>3</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>44440</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>44470</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>103</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>44501</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>104</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>44531</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
         <v>91</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>44562</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="14" t="s">
         <v>92</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="14" t="s">
         <v>55</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>44621</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="14" t="s">
         <v>99</v>
       </c>
@@ -1543,18 +1543,14 @@
         <v>44652</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>96</v>
-      </c>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="14"/>
+      <c r="B52" s="7"/>
       <c r="C52" s="16">
         <v>44682</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A53" s="14" t="s">
         <v>93</v>
       </c>
@@ -1565,7 +1561,7 @@
         <v>44713</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="12" t="s">
         <v>100</v>
       </c>
@@ -1576,7 +1572,7 @@
         <v>44743</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="12" t="s">
         <v>3</v>
       </c>
@@ -1587,7 +1583,7 @@
         <v>44805</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
         <v>65</v>
       </c>
@@ -1598,7 +1594,7 @@
         <v>44835</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
         <v>6</v>
       </c>
@@ -1609,7 +1605,7 @@
         <v>44866</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>47</v>
       </c>
@@ -1620,18 +1616,10 @@
         <v>44896</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>106</v>
-      </c>
-      <c r="B59" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="C59" s="16">
-        <v>44927</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B59" s="13"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>30</v>
       </c>
@@ -1642,18 +1630,18 @@
         <v>44958</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C61" s="16">
         <v>44986</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>92</v>
       </c>
@@ -1664,9 +1652,9 @@
         <v>45017</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>102</v>
@@ -1675,9 +1663,9 @@
         <v>45047</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>101</v>
@@ -1686,42 +1674,42 @@
         <v>45078</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>112</v>
+      </c>
+      <c r="B65" s="13" t="s">
         <v>113</v>
-      </c>
-      <c r="B65" s="13" t="s">
-        <v>114</v>
       </c>
       <c r="C65" s="16">
         <v>45108</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>110</v>
+      </c>
+      <c r="B66" s="13" t="s">
         <v>111</v>
-      </c>
-      <c r="B66" s="13" t="s">
-        <v>112</v>
       </c>
       <c r="C66" s="16">
         <v>45170</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>65</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C67" s="16">
         <v>45200</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>43</v>
@@ -1730,9 +1718,9 @@
         <v>45231</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>98</v>
@@ -1741,7 +1729,7 @@
         <v>45261</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>3</v>
       </c>
@@ -1752,40 +1740,40 @@
         <v>45292</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>117</v>
+      </c>
+      <c r="B71" s="15" t="s">
         <v>118</v>
-      </c>
-      <c r="B71" s="15" t="s">
-        <v>119</v>
       </c>
       <c r="C71" s="16">
         <v>45323</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C72" s="16">
         <v>45352</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>3</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C73" s="16">
         <v>45383</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>8</v>
       </c>
@@ -1796,84 +1784,84 @@
         <v>45413</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B75" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C75" s="16">
         <v>45444</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>7</v>
+        <v>132</v>
       </c>
       <c r="C76" s="16">
         <v>45474</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="14" t="s">
         <v>93</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C77" s="16">
         <v>45536</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B78" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C78" s="16">
         <v>45566</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B79" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C79" s="16">
         <v>45597</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B80" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C80" s="16">
         <v>45627</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>130</v>
+      </c>
+      <c r="B81" t="s">
         <v>131</v>
-      </c>
-      <c r="B81" t="s">
-        <v>132</v>
       </c>
       <c r="C81" s="16">
         <v>45658</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="14" t="s">
         <v>99</v>
       </c>
@@ -1884,7 +1872,7 @@
         <v>45689</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="14" t="s">
         <v>99</v>
       </c>
@@ -1915,7 +1903,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1931,7 +1919,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>